<commit_message>
ICEM makale figürleri (drive) eklendi.
</commit_message>
<xml_diff>
--- a/Paper/ICEM 2018/Results/icem_results.xlsx
+++ b/Paper/ICEM 2018/Results/icem_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16524" windowHeight="5628"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16530" windowHeight="5625"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>2L-IGBT</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>10uF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/epcos-tdk/B32676E3206K000/495-2952-ND/1277716</t>
+  </si>
+  <si>
+    <t>20uF</t>
   </si>
 </sst>
 </file>
@@ -548,20 +554,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="85.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="85.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -587,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -625,7 +631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -663,7 +669,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -701,7 +707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -739,7 +745,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -777,7 +783,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -806,7 +812,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -832,11 +838,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="7">
+        <v>4.8199999999999996E-3</v>
+      </c>
       <c r="C9" s="7">
         <v>9.8300000000000002E-3</v>
       </c>
@@ -856,11 +864,13 @@
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="7">
+        <v>0.79910000000000003</v>
+      </c>
       <c r="C10" s="7">
         <v>0.89149999999999996</v>
       </c>
@@ -879,8 +889,17 @@
       <c r="H10" s="7">
         <v>0.89149999999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
     </row>
   </sheetData>
@@ -890,8 +909,9 @@
     <hyperlink ref="M4" r:id="rId3"/>
     <hyperlink ref="M5" r:id="rId4"/>
     <hyperlink ref="M6" r:id="rId5"/>
+    <hyperlink ref="M10" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>